<commit_message>
updated workflow. all new files
</commit_message>
<xml_diff>
--- a/Data/Raw/Pn_Ex2_Chlorophyll.xlsx
+++ b/Data/Raw/Pn_Ex2_Chlorophyll.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zacharyquinlan/Documents/GitHub/pseudonitzschia_Koester/Data/Raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A3B5975-4530-FC48-8FFF-B4D4FF87C233}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CA9AB8-0DDB-B946-9656-BD5628DEAAFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="19400" windowHeight="10400" xr2:uid="{70A6565A-C6B5-4BD3-96AB-EEAE66632E0F}"/>
   </bookViews>
@@ -48,9 +48,6 @@
     <t>Pn_subpacifica_A</t>
   </si>
   <si>
-    <t>Pn_ subpacifica_B</t>
-  </si>
-  <si>
     <t>Pn_galaxiae_A</t>
   </si>
   <si>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>chl</t>
+  </si>
+  <si>
+    <t>Pn_subpacifica_B</t>
   </si>
 </sst>
 </file>
@@ -422,7 +422,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -432,10 +432,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -480,7 +480,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B7">
         <v>18.84</v>
@@ -488,7 +488,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>156.37</v>
@@ -496,7 +496,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>193.17</v>
@@ -504,7 +504,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10">
         <v>222.42</v>
@@ -512,7 +512,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11">
         <v>254.32</v>

</xml_diff>